<commit_message>
Moack serial input complete, api call code there, starting on LCD
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Current Projects\Part Weight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Craig\Documents\GitHubVisualStudio\PythonScale\PythonScale\DocsANdNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
+    <workbookView xWindow="2040" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LED Status" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Power</t>
   </si>
@@ -253,18 +253,6 @@
   </si>
   <si>
     <t>GPIO26</t>
-  </si>
-  <si>
-    <t>GPIO13</t>
-  </si>
-  <si>
-    <t>GPIO21</t>
-  </si>
-  <si>
-    <t>GPIO16</t>
-  </si>
-  <si>
-    <t>GPIO20</t>
   </si>
   <si>
     <t>GPIO12</t>
@@ -1062,7 +1050,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1110,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>51</v>
@@ -1133,10 +1121,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>33</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>35</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>51</v>
@@ -1147,10 +1135,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>51</v>
@@ -1161,10 +1149,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
-        <v>36</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>78</v>
+        <v>33</v>
+      </c>
+      <c r="B8" s="12">
+        <v>13</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>51</v>
@@ -1175,10 +1163,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
-        <v>37</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>75</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="12">
+        <v>16</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>51</v>
@@ -1191,8 +1179,8 @@
       <c r="A10" s="11">
         <v>38</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>79</v>
+      <c r="B10" s="12">
+        <v>20</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>51</v>
@@ -1205,8 +1193,8 @@
       <c r="A11" s="14">
         <v>40</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>77</v>
+      <c r="B11" s="15">
+        <v>21</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>51</v>
@@ -1220,7 +1208,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Refactered, added 3 NoGo LEDs, added functions for easily controlling all LEDs (blink, cycle through, etc)
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
+    <workbookView xWindow="3150" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LED Status" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
   <si>
     <t>Power</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Pi Pins</t>
   </si>
   <si>
-    <t>Pin #</t>
-  </si>
-  <si>
     <t>LCD Pin 6, Clock En</t>
   </si>
   <si>
@@ -234,28 +231,43 @@
     <t>Serial Tx</t>
   </si>
   <si>
-    <t>Pin Name</t>
-  </si>
-  <si>
     <t>RXD0</t>
   </si>
   <si>
     <t>TXD0</t>
   </si>
   <si>
-    <t>GPIO19</t>
-  </si>
-  <si>
-    <t>GPIO05</t>
-  </si>
-  <si>
-    <t>GPIO06</t>
-  </si>
-  <si>
-    <t>GPIO26</t>
-  </si>
-  <si>
-    <t>GPIO12</t>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Serial</t>
+  </si>
+  <si>
+    <t>SPI MOSI</t>
+  </si>
+  <si>
+    <t>SPI CE1</t>
+  </si>
+  <si>
+    <t>SPI CE0</t>
+  </si>
+  <si>
+    <t>SPI MISO</t>
+  </si>
+  <si>
+    <t>SPI CLK</t>
+  </si>
+  <si>
+    <t>Go Led</t>
+  </si>
+  <si>
+    <t>NoGo Led 1</t>
+  </si>
+  <si>
+    <t>NoGo Led 2</t>
+  </si>
+  <si>
+    <t>NoGo Led 3</t>
   </si>
 </sst>
 </file>
@@ -315,15 +327,39 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -347,17 +383,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -378,32 +403,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -430,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,15 +454,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,12 +477,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9966FF"/>
+      <color rgb="FF9900FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -775,16 +798,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
@@ -804,16 +827,16 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -833,12 +856,12 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
@@ -849,12 +872,12 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
@@ -867,12 +890,12 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
@@ -890,12 +913,12 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="19"/>
+      <c r="C7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
@@ -908,10 +931,10 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
@@ -924,10 +947,10 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22" t="s">
+      <c r="B9" s="19"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -947,12 +970,12 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -967,12 +990,12 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -992,12 +1015,12 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1015,12 +1038,12 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1047,227 +1070,369 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F18" sqref="F18:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="21">
+        <v>2</v>
+      </c>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>12</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="21">
+        <v>3</v>
+      </c>
+      <c r="F5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>19</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="23">
+        <v>4</v>
+      </c>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>26</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>29</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="E7" s="23">
+        <v>5</v>
+      </c>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="23">
+        <v>6</v>
+      </c>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="27">
+        <v>7</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>20</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
-        <v>31</v>
-      </c>
-      <c r="B4" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="27">
+        <v>8</v>
+      </c>
+      <c r="F10" s="28"/>
+      <c r="G10" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="12" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>21</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>32</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>35</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
-        <v>37</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="C11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="27">
+        <v>9</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
-        <v>33</v>
-      </c>
-      <c r="B8" s="12">
-        <v>13</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="13" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>17</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
-        <v>36</v>
-      </c>
-      <c r="B9" s="12">
-        <v>16</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>38</v>
-      </c>
-      <c r="B10" s="12">
-        <v>20</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>40</v>
-      </c>
-      <c r="B11" s="15">
-        <v>21</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>32</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>76</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="27">
+        <v>10</v>
+      </c>
+      <c r="F12" s="28"/>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>18</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="27">
+        <v>11</v>
+      </c>
+      <c r="F13" s="28"/>
+      <c r="G13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="23">
+        <v>12</v>
+      </c>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="23">
+        <v>13</v>
+      </c>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="25">
+        <v>14</v>
+      </c>
+      <c r="F16" s="26" t="str">
+        <f>C14</f>
+        <v>Serial Rx</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="25">
+        <v>15</v>
+      </c>
+      <c r="F17" s="26" t="str">
+        <f>C15</f>
+        <v>Serial Tx</v>
+      </c>
+      <c r="G17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>31</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>10</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
-        <v>8</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13" t="s">
-        <v>65</v>
+      <c r="E18" s="23">
+        <v>16</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="23">
+        <v>17</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="23">
+        <v>18</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="23">
+        <v>19</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="23">
+        <v>20</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="23">
+        <v>21</v>
+      </c>
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="23">
+        <v>22</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="23">
+        <v>23</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="23">
+        <v>24</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="23">
+        <v>25</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="23">
+        <v>26</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="23">
+        <v>27</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored out Button Config and created a Button class
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Power</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>NoGo Led 3</t>
+  </si>
+  <si>
+    <t>btn Exit</t>
+  </si>
+  <si>
+    <t>btn Reset</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1079,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:F19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,7 +1162,9 @@
       <c r="E6" s="23">
         <v>4</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="24" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
@@ -1171,7 +1179,9 @@
       <c r="E7" s="23">
         <v>5</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="24" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10">

</xml_diff>

<commit_message>
Add physical pins to table
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -298,7 +298,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,8 +357,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +404,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,6 +554,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1123,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,20 +1582,20 @@
       </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="29">
+      <c r="E34" s="33">
         <v>2</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="29" t="s">
+      <c r="F34" s="34"/>
+      <c r="G34" s="33" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="29">
+      <c r="E35" s="33">
         <v>4</v>
       </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="29" t="s">
+      <c r="F35" s="34"/>
+      <c r="G35" s="33" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed Pin numbers in the code
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cverburgh\Documents\Visual Studio 2015\Projects\PythonScale\PythonScale\DocsANdNotes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Craig\Documents\GitHubVisualStudio\PythonScale\PythonScale\DocsANdNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="2"/>
+    <workbookView xWindow="7410" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LED Status" sheetId="1" r:id="rId1"/>
@@ -373,15 +373,9 @@
     <t>PI Pin</t>
   </si>
   <si>
-    <t>NoGo LED 2</t>
-  </si>
-  <si>
     <t>LCD Pin 12, Data 05</t>
   </si>
   <si>
-    <t>NoGo LED 3</t>
-  </si>
-  <si>
     <t>LCD Pin 13, Data 06</t>
   </si>
   <si>
@@ -446,6 +440,12 @@
   </si>
   <si>
     <t>LCD Pin 03, To Pot</t>
+  </si>
+  <si>
+    <t>LED - NoGo 2</t>
+  </si>
+  <si>
+    <t>LED - NoGo 3</t>
   </si>
 </sst>
 </file>
@@ -744,9 +744,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -826,6 +823,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1249,12 +1249,12 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
       <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1431,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O42"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:K25"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1512,32 +1512,32 @@
       <c r="C6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="32">
         <v>1</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="33">
         <v>2</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="M6" s="38">
+      <c r="M6" s="37">
         <v>11</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="49" t="s">
-        <v>124</v>
+      <c r="O6" s="48" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1550,30 +1550,30 @@
       <c r="C7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="35" t="s">
+      <c r="F7" s="41"/>
+      <c r="G7" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="35">
         <v>3</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="33">
         <v>4</v>
       </c>
-      <c r="J7" s="34" t="s">
+      <c r="J7" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="M7" s="38">
+      <c r="K7" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="M7" s="37">
         <v>13</v>
       </c>
-      <c r="N7" s="38" t="s">
+      <c r="N7" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="O7" s="49" t="s">
-        <v>125</v>
+      <c r="O7" s="48" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -1586,30 +1586,30 @@
       <c r="C8" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="35" t="s">
+      <c r="F8" s="41"/>
+      <c r="G8" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>5</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="36">
         <v>6</v>
       </c>
-      <c r="J8" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="M8" s="38">
+      <c r="J8" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="M8" s="37">
         <v>15</v>
       </c>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="49" t="s">
-        <v>126</v>
+      <c r="O8" s="48" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1620,29 +1620,29 @@
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="38" t="s">
+      <c r="F9" s="41"/>
+      <c r="G9" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="37">
         <v>7</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="38">
         <v>8</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="32">
         <v>1</v>
       </c>
-      <c r="N9" s="33" t="s">
+      <c r="N9" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="O9" s="51" t="s">
+      <c r="O9" s="50" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1654,28 +1654,28 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="37">
+      <c r="G10" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="36">
         <v>9</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="38">
         <v>10</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="47" t="s">
+      <c r="K10" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="32">
         <v>17</v>
       </c>
-      <c r="N10" s="33" t="s">
+      <c r="N10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="51" t="s">
+      <c r="O10" s="50" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1687,30 +1687,30 @@
       <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="37">
         <v>11</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="37">
         <v>12</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="J11" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="M11" s="37">
+      <c r="K11" s="47"/>
+      <c r="M11" s="36">
         <v>14</v>
       </c>
-      <c r="N11" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" s="52" t="s">
-        <v>122</v>
+      <c r="N11" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="51" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1721,32 +1721,32 @@
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="37">
         <v>13</v>
       </c>
-      <c r="I12" s="37">
+      <c r="I12" s="36">
         <v>14</v>
       </c>
-      <c r="J12" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="46" t="s">
+      <c r="J12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="34">
+      <c r="M12" s="33">
         <v>4</v>
       </c>
-      <c r="N12" s="34" t="s">
+      <c r="N12" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="O12" s="45" t="s">
-        <v>121</v>
+      <c r="O12" s="44" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -1757,28 +1757,28 @@
       <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="37">
         <v>15</v>
       </c>
-      <c r="I13" s="38">
+      <c r="I13" s="37">
         <v>16</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="49" t="s">
+      <c r="K13" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="48" t="s">
-        <v>138</v>
+      <c r="M13" s="31"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="47" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -1786,32 +1786,32 @@
         <v>12</v>
       </c>
       <c r="C14" s="20"/>
-      <c r="F14" s="42" t="s">
+      <c r="F14" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="33">
+      <c r="H14" s="32">
         <v>17</v>
       </c>
-      <c r="I14" s="38">
+      <c r="I14" s="37">
         <v>18</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="49" t="s">
+      <c r="K14" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="38">
+      <c r="M14" s="37">
         <v>16</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="N14" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="O14" s="49" t="s">
-        <v>129</v>
+      <c r="O14" s="48" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1819,28 +1819,28 @@
         <v>13</v>
       </c>
       <c r="C15" s="20"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="40" t="s">
+      <c r="F15" s="41"/>
+      <c r="G15" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="39">
         <v>19</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="36">
         <v>20</v>
       </c>
-      <c r="J15" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="48"/>
-      <c r="M15" s="37">
+      <c r="J15" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="47"/>
+      <c r="M15" s="36">
         <v>6</v>
       </c>
-      <c r="N15" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O15" s="46" t="s">
-        <v>137</v>
+      <c r="N15" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="45" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1856,28 +1856,28 @@
       <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="40" t="s">
+      <c r="F16" s="41"/>
+      <c r="G16" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="39">
         <v>21</v>
       </c>
-      <c r="I16" s="38">
+      <c r="I16" s="37">
         <v>22</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="48"/>
-      <c r="M16" s="38">
+      <c r="K16" s="47"/>
+      <c r="M16" s="37">
         <v>18</v>
       </c>
-      <c r="N16" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="O16" s="49" t="s">
-        <v>128</v>
+      <c r="N16" s="37" t="s">
+        <v>125</v>
+      </c>
+      <c r="O16" s="48" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1893,28 +1893,28 @@
       <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="40" t="s">
+      <c r="F17" s="41"/>
+      <c r="G17" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="39">
         <v>23</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="39">
         <v>24</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="K17" s="48"/>
-      <c r="M17" s="38">
+      <c r="K17" s="47"/>
+      <c r="M17" s="37">
         <v>32</v>
       </c>
-      <c r="N17" s="38" t="s">
+      <c r="N17" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="O17" s="49" t="s">
-        <v>132</v>
+      <c r="O17" s="48" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1927,28 +1927,28 @@
       <c r="C18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="37">
+      <c r="F18" s="41"/>
+      <c r="G18" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="36">
         <v>25</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="39">
         <v>26</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="48"/>
-      <c r="M18" s="38">
+      <c r="K18" s="47"/>
+      <c r="M18" s="37">
         <v>36</v>
       </c>
-      <c r="N18" s="38" t="s">
+      <c r="N18" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="49" t="s">
-        <v>116</v>
+      <c r="O18" s="48" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1961,28 +1961,28 @@
       <c r="C19" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="41" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="41">
+      <c r="H19" s="40">
         <v>27</v>
       </c>
-      <c r="I19" s="41">
+      <c r="I19" s="40">
         <v>28</v>
       </c>
-      <c r="J19" s="41" t="s">
+      <c r="J19" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="K19" s="48"/>
-      <c r="M19" s="38">
+      <c r="K19" s="47"/>
+      <c r="M19" s="37">
         <v>38</v>
       </c>
-      <c r="N19" s="38" t="s">
+      <c r="N19" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="O19" s="49" t="s">
-        <v>118</v>
+      <c r="O19" s="48" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1995,32 +1995,32 @@
       <c r="C20" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="38" t="s">
+      <c r="G20" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="37">
         <v>29</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="36">
         <v>30</v>
       </c>
-      <c r="J20" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K20" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="M20" s="38">
+      <c r="J20" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="M20" s="37">
         <v>40</v>
       </c>
-      <c r="N20" s="38" t="s">
+      <c r="N20" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="O20" s="49" t="s">
-        <v>119</v>
+      <c r="O20" s="48" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -2033,32 +2033,32 @@
       <c r="C21" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="G21" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="38">
+      <c r="H21" s="37">
         <v>31</v>
       </c>
-      <c r="I21" s="38">
+      <c r="I21" s="37">
         <v>32</v>
       </c>
-      <c r="J21" s="38" t="s">
+      <c r="J21" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="K21" s="49" t="s">
+      <c r="K21" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="M21" s="34">
+      <c r="M21" s="33">
         <v>2</v>
       </c>
-      <c r="N21" s="34" t="s">
+      <c r="N21" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="O21" s="45" t="s">
-        <v>120</v>
+      <c r="O21" s="44" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -2071,30 +2071,30 @@
       <c r="C22" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="38" t="s">
+      <c r="G22" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="38">
+      <c r="H22" s="37">
         <v>33</v>
       </c>
-      <c r="I22" s="37">
+      <c r="I22" s="36">
         <v>34</v>
       </c>
-      <c r="J22" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="K22" s="44"/>
-      <c r="M22" s="37">
+      <c r="J22" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="43"/>
+      <c r="M22" s="36">
         <v>30</v>
       </c>
-      <c r="N22" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O22" s="46" t="s">
-        <v>135</v>
+      <c r="N22" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O22" s="45" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -2102,32 +2102,32 @@
         <v>21</v>
       </c>
       <c r="C23" s="20"/>
-      <c r="F23" s="43" t="s">
+      <c r="F23" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="38">
+      <c r="H23" s="37">
         <v>35</v>
       </c>
-      <c r="I23" s="38">
+      <c r="I23" s="37">
         <v>36</v>
       </c>
-      <c r="J23" s="38" t="s">
+      <c r="J23" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="49" t="s">
+      <c r="K23" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="38">
+      <c r="M23" s="37">
         <v>31</v>
       </c>
-      <c r="N23" s="38" t="s">
+      <c r="N23" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="O23" s="49" t="s">
-        <v>131</v>
+      <c r="O23" s="48" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -2140,32 +2140,32 @@
       <c r="C24" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="38">
+      <c r="H24" s="37">
         <v>37</v>
       </c>
-      <c r="I24" s="38">
+      <c r="I24" s="37">
         <v>38</v>
       </c>
-      <c r="J24" s="38" t="s">
+      <c r="J24" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="M24" s="38">
+      <c r="M24" s="37">
         <v>33</v>
       </c>
-      <c r="N24" s="38" t="s">
+      <c r="N24" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="O24" s="49" t="s">
-        <v>133</v>
+      <c r="O24" s="48" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -2178,30 +2178,30 @@
       <c r="C25" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="42"/>
-      <c r="G25" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="37">
+      <c r="F25" s="41"/>
+      <c r="G25" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="36">
         <v>39</v>
       </c>
-      <c r="I25" s="38">
+      <c r="I25" s="37">
         <v>40</v>
       </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="K25" s="49" t="s">
+      <c r="K25" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="38">
-        <v>29</v>
-      </c>
-      <c r="N25" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="O25" s="49" t="s">
-        <v>130</v>
+      <c r="M25" s="37">
+        <v>35</v>
+      </c>
+      <c r="N25" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="O25" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2214,15 +2214,15 @@
       <c r="C26" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K26" s="44"/>
-      <c r="M26" s="38">
-        <v>35</v>
-      </c>
-      <c r="N26" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="O26" s="49" t="s">
-        <v>115</v>
+      <c r="K26" s="43"/>
+      <c r="M26" s="37">
+        <v>37</v>
+      </c>
+      <c r="N26" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="O26" s="48" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2236,14 +2236,14 @@
         <v>54</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="M27" s="38">
-        <v>37</v>
-      </c>
-      <c r="N27" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="O27" s="49" t="s">
-        <v>117</v>
+      <c r="M27" s="37">
+        <v>29</v>
+      </c>
+      <c r="N27" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="48" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2257,14 +2257,14 @@
         <v>52</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="M28" s="39">
+      <c r="M28" s="38">
         <v>10</v>
       </c>
-      <c r="N28" s="39" t="s">
+      <c r="N28" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="O28" s="47" t="s">
-        <v>123</v>
+      <c r="O28" s="46" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2278,162 +2278,162 @@
         <v>53</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="M29" s="39">
+      <c r="M29" s="38">
         <v>8</v>
       </c>
-      <c r="N29" s="39" t="s">
+      <c r="N29" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="O29" s="47" t="s">
+      <c r="O29" s="46" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K30" s="1"/>
-      <c r="M30" s="37">
+      <c r="M30" s="36">
         <v>9</v>
       </c>
-      <c r="N30" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O30" s="46"/>
+      <c r="N30" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O30" s="45"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>73</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="M31" s="37">
+      <c r="M31" s="36">
         <v>20</v>
       </c>
-      <c r="N31" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O31" s="46"/>
+      <c r="N31" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O31" s="45"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="26">
+      <c r="A32" s="25">
         <v>1</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="26" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="25" t="s">
         <v>76</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="M32" s="37">
+      <c r="M32" s="36">
         <v>25</v>
       </c>
-      <c r="N32" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O32" s="46"/>
+      <c r="N32" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O32" s="45"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="26">
+      <c r="A33" s="25">
         <v>17</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="26"/>
+      <c r="C33" s="25" t="s">
         <v>76</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="M33" s="37">
+      <c r="M33" s="36">
         <v>34</v>
       </c>
-      <c r="N33" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="O33" s="46"/>
+      <c r="N33" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="O33" s="45"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="30">
+      <c r="A34" s="29">
         <v>2</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="30" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="29" t="s">
         <v>75</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="M34" s="50">
+      <c r="M34" s="49">
         <v>39</v>
       </c>
-      <c r="N34" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="O34" s="52"/>
+      <c r="N34" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="O34" s="51"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="30">
+      <c r="A35" s="29">
         <v>4</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="30" t="s">
+      <c r="B35" s="30"/>
+      <c r="C35" s="29" t="s">
         <v>75</v>
       </c>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="28">
+      <c r="A36" s="27">
         <v>6</v>
       </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="28" t="s">
+      <c r="B36" s="28"/>
+      <c r="C36" s="27" t="s">
         <v>74</v>
       </c>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="28">
+      <c r="A37" s="27">
         <v>9</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="28" t="s">
+      <c r="B37" s="28"/>
+      <c r="C37" s="27" t="s">
         <v>74</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="28">
+      <c r="A38" s="27">
         <v>14</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="28" t="s">
+      <c r="B38" s="28"/>
+      <c r="C38" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="28">
+      <c r="A39" s="27">
         <v>20</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="28" t="s">
+      <c r="B39" s="28"/>
+      <c r="C39" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="A40" s="27">
         <v>25</v>
       </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="28" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="28">
+      <c r="A41" s="27">
         <v>30</v>
       </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="28" t="s">
+      <c r="B41" s="28"/>
+      <c r="C41" s="27" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="28">
+      <c r="A42" s="27">
         <v>39</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="28" t="s">
+      <c r="B42" s="28"/>
+      <c r="C42" s="27" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2450,7 +2450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="L10:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
@@ -2468,146 +2468,146 @@
   </cols>
   <sheetData>
     <row r="10" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L10" s="42" t="s">
+      <c r="L10" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="33" t="s">
+      <c r="M10" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="33">
+      <c r="N10" s="32">
         <v>1</v>
       </c>
-      <c r="O10" s="34">
+      <c r="O10" s="33">
         <v>2</v>
       </c>
-      <c r="P10" s="34" t="s">
+      <c r="P10" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="45" t="s">
+      <c r="Q10" s="44" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L11" s="42"/>
-      <c r="M11" s="35" t="s">
+      <c r="L11" s="41"/>
+      <c r="M11" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="35">
         <v>3</v>
       </c>
-      <c r="O11" s="34">
+      <c r="O11" s="33">
         <v>4</v>
       </c>
-      <c r="P11" s="34" t="s">
+      <c r="P11" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="45" t="s">
-        <v>136</v>
+      <c r="Q11" s="44" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L12" s="42"/>
-      <c r="M12" s="35" t="s">
+      <c r="L12" s="41"/>
+      <c r="M12" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="35">
         <v>5</v>
       </c>
-      <c r="O12" s="37">
+      <c r="O12" s="36">
         <v>6</v>
       </c>
-      <c r="P12" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q12" s="46" t="s">
+      <c r="P12" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="45" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L13" s="41"/>
+      <c r="M13" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="37">
+        <v>7</v>
+      </c>
+      <c r="O13" s="38">
+        <v>8</v>
+      </c>
+      <c r="P13" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q13" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="X13" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y13" s="52"/>
+      <c r="Z13" s="10"/>
+    </row>
+    <row r="14" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="M14" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14" s="36">
+        <v>9</v>
+      </c>
+      <c r="O14" s="38">
+        <v>10</v>
+      </c>
+      <c r="P14" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q14" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="X14" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y14" s="52"/>
+      <c r="AA14" s="53"/>
+    </row>
+    <row r="15" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L15" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="37">
+        <v>11</v>
+      </c>
+      <c r="O15" s="37">
+        <v>12</v>
+      </c>
+      <c r="P15" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q15" s="47"/>
+      <c r="X15" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="13" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L13" s="42"/>
-      <c r="M13" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="N13" s="38">
-        <v>7</v>
-      </c>
-      <c r="O13" s="39">
-        <v>8</v>
-      </c>
-      <c r="P13" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q13" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="X13" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y13" s="53"/>
-      <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="M14" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N14" s="37">
-        <v>9</v>
-      </c>
-      <c r="O14" s="39">
-        <v>10</v>
-      </c>
-      <c r="P14" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q14" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="X14" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="Y14" s="53"/>
-      <c r="AA14" s="54"/>
-    </row>
-    <row r="15" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L15" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="M15" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="N15" s="38">
-        <v>11</v>
-      </c>
-      <c r="O15" s="38">
-        <v>12</v>
-      </c>
-      <c r="P15" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q15" s="48"/>
-      <c r="X15" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z15" s="54"/>
-      <c r="AA15" s="54"/>
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="53"/>
     </row>
     <row r="16" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L16" s="43" t="s">
+      <c r="L16" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="M16" s="38" t="s">
+      <c r="M16" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="N16" s="38">
+      <c r="N16" s="37">
         <v>13</v>
       </c>
-      <c r="O16" s="37">
+      <c r="O16" s="36">
         <v>14</v>
       </c>
-      <c r="P16" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" s="46" t="s">
+      <c r="P16" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" s="45" t="s">
         <v>110</v>
       </c>
       <c r="S16" s="10"/>
@@ -2615,55 +2615,55 @@
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
       <c r="W16" s="11"/>
-      <c r="X16" s="49" t="s">
+      <c r="X16" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="Z16" s="54"/>
-      <c r="AA16" s="54"/>
+      <c r="Z16" s="53"/>
+      <c r="AA16" s="53"/>
     </row>
     <row r="17" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L17" s="43" t="s">
+      <c r="L17" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="38" t="s">
+      <c r="M17" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="38">
+      <c r="N17" s="37">
         <v>15</v>
       </c>
-      <c r="O17" s="38">
+      <c r="O17" s="37">
         <v>16</v>
       </c>
-      <c r="P17" s="38" t="s">
+      <c r="P17" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="Q17" s="49" t="s">
+      <c r="Q17" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="R17" s="55"/>
-      <c r="X17" s="46" t="s">
-        <v>137</v>
-      </c>
-      <c r="Z17" s="54"/>
-      <c r="AA17" s="54"/>
+      <c r="R17" s="54"/>
+      <c r="X17" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
     </row>
     <row r="18" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L18" s="42" t="s">
+      <c r="L18" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="M18" s="33" t="s">
+      <c r="M18" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="N18" s="33">
+      <c r="N18" s="32">
         <v>17</v>
       </c>
-      <c r="O18" s="38">
+      <c r="O18" s="37">
         <v>18</v>
       </c>
-      <c r="P18" s="38" t="s">
+      <c r="P18" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="Q18" s="49" t="s">
+      <c r="Q18" s="48" t="s">
         <v>51</v>
       </c>
       <c r="R18" s="10"/>
@@ -2672,156 +2672,156 @@
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="11"/>
-      <c r="X18" s="49" t="s">
+      <c r="X18" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="Z18" s="54"/>
-      <c r="AA18" s="54"/>
+      <c r="Z18" s="53"/>
+      <c r="AA18" s="53"/>
     </row>
     <row r="19" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L19" s="42"/>
-      <c r="M19" s="40" t="s">
+      <c r="L19" s="41"/>
+      <c r="M19" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="40">
+      <c r="N19" s="39">
         <v>19</v>
       </c>
-      <c r="O19" s="37">
+      <c r="O19" s="36">
         <v>20</v>
       </c>
-      <c r="P19" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q19" s="48"/>
-      <c r="Z19" s="54"/>
-      <c r="AA19" s="54"/>
+      <c r="P19" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q19" s="47"/>
+      <c r="Z19" s="53"/>
+      <c r="AA19" s="53"/>
     </row>
     <row r="20" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L20" s="42"/>
-      <c r="M20" s="40" t="s">
+      <c r="L20" s="41"/>
+      <c r="M20" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="N20" s="40">
+      <c r="N20" s="39">
         <v>21</v>
       </c>
-      <c r="O20" s="38">
+      <c r="O20" s="37">
         <v>22</v>
       </c>
-      <c r="P20" s="38" t="s">
+      <c r="P20" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="Q20" s="48"/>
-      <c r="Z20" s="54"/>
-      <c r="AA20" s="54"/>
+      <c r="Q20" s="47"/>
+      <c r="Z20" s="53"/>
+      <c r="AA20" s="53"/>
     </row>
     <row r="21" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L21" s="42"/>
-      <c r="M21" s="40" t="s">
+      <c r="L21" s="41"/>
+      <c r="M21" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="N21" s="40">
+      <c r="N21" s="39">
         <v>23</v>
       </c>
-      <c r="O21" s="40">
+      <c r="O21" s="39">
         <v>24</v>
       </c>
-      <c r="P21" s="40" t="s">
+      <c r="P21" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="Q21" s="48"/>
-      <c r="Z21" s="54"/>
-      <c r="AA21" s="54"/>
+      <c r="Q21" s="47"/>
+      <c r="Z21" s="53"/>
+      <c r="AA21" s="53"/>
     </row>
     <row r="22" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L22" s="42"/>
-      <c r="M22" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N22" s="37">
+      <c r="L22" s="41"/>
+      <c r="M22" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" s="36">
         <v>25</v>
       </c>
-      <c r="O22" s="40">
+      <c r="O22" s="39">
         <v>26</v>
       </c>
-      <c r="P22" s="40" t="s">
+      <c r="P22" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="Q22" s="48"/>
-      <c r="Z22" s="54"/>
-      <c r="AA22" s="54"/>
+      <c r="Q22" s="47"/>
+      <c r="Z22" s="53"/>
+      <c r="AA22" s="53"/>
     </row>
     <row r="23" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L23" s="42"/>
-      <c r="M23" s="41" t="s">
+      <c r="L23" s="41"/>
+      <c r="M23" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="N23" s="41">
+      <c r="N23" s="40">
         <v>27</v>
       </c>
-      <c r="O23" s="41">
+      <c r="O23" s="40">
         <v>28</v>
       </c>
-      <c r="P23" s="41" t="s">
+      <c r="P23" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="Q23" s="48"/>
+      <c r="Q23" s="47"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
       <c r="W23" s="11"/>
-      <c r="X23" s="49" t="s">
+      <c r="X23" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="Z23" s="54"/>
-      <c r="AA23" s="54"/>
+      <c r="Z23" s="53"/>
+      <c r="AA23" s="53"/>
     </row>
     <row r="24" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L24" s="43" t="s">
+      <c r="L24" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="M24" s="38" t="s">
+      <c r="M24" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="N24" s="38">
+      <c r="N24" s="37">
         <v>29</v>
       </c>
-      <c r="O24" s="37">
+      <c r="O24" s="36">
         <v>30</v>
       </c>
-      <c r="P24" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q24" s="59" t="s">
-        <v>134</v>
+      <c r="P24" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24" s="58" t="s">
+        <v>132</v>
       </c>
       <c r="R24" s="8"/>
       <c r="S24" s="9"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
       <c r="W24" s="11"/>
-      <c r="X24" s="49" t="s">
+      <c r="X24" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="Z24" s="54"/>
-      <c r="AA24" s="54"/>
+      <c r="Z24" s="53"/>
+      <c r="AA24" s="53"/>
     </row>
     <row r="25" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L25" s="43" t="s">
+      <c r="L25" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="M25" s="38" t="s">
+      <c r="M25" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="N25" s="38">
+      <c r="N25" s="37">
         <v>31</v>
       </c>
-      <c r="O25" s="38">
+      <c r="O25" s="37">
         <v>32</v>
       </c>
-      <c r="P25" s="38" t="s">
+      <c r="P25" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="Q25" s="58" t="s">
+      <c r="Q25" s="57" t="s">
         <v>55</v>
       </c>
       <c r="R25" s="10"/>
@@ -2829,117 +2829,117 @@
       <c r="T25" s="9"/>
       <c r="V25" s="10"/>
       <c r="W25" s="11"/>
-      <c r="X25" s="49" t="s">
+      <c r="X25" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="Z25" s="54"/>
-      <c r="AA25" s="54"/>
+      <c r="Z25" s="53"/>
+      <c r="AA25" s="53"/>
     </row>
     <row r="26" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L26" s="43" t="s">
+      <c r="L26" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="M26" s="38" t="s">
+      <c r="M26" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="N26" s="38">
+      <c r="N26" s="37">
         <v>33</v>
       </c>
-      <c r="O26" s="37">
+      <c r="O26" s="36">
         <v>34</v>
       </c>
-      <c r="P26" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q26" s="44"/>
+      <c r="P26" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q26" s="43"/>
       <c r="T26" s="9"/>
-      <c r="V26" s="56"/>
+      <c r="V26" s="55"/>
       <c r="W26" s="11"/>
-      <c r="X26" s="49" t="s">
+      <c r="X26" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="Z26" s="54"/>
-      <c r="AA26" s="54"/>
+      <c r="Z26" s="53"/>
+      <c r="AA26" s="53"/>
     </row>
     <row r="27" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L27" s="43" t="s">
+      <c r="L27" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="M27" s="38" t="s">
+      <c r="M27" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="N27" s="38">
+      <c r="N27" s="37">
         <v>35</v>
       </c>
-      <c r="O27" s="38">
+      <c r="O27" s="37">
         <v>36</v>
       </c>
-      <c r="P27" s="38" t="s">
+      <c r="P27" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="Q27" s="49" t="s">
+      <c r="Q27" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="53"/>
+      <c r="R27" s="52"/>
       <c r="S27" s="10"/>
       <c r="T27" s="11"/>
-      <c r="V27" s="57"/>
-      <c r="X27" s="45" t="s">
+      <c r="V27" s="56"/>
+      <c r="X27" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="Y27" s="53"/>
-      <c r="Z27" s="54"/>
-      <c r="AA27" s="54"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="53"/>
+      <c r="AA27" s="53"/>
     </row>
     <row r="28" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L28" s="43" t="s">
+      <c r="L28" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="M28" s="38" t="s">
+      <c r="M28" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="N28" s="38">
+      <c r="N28" s="37">
         <v>37</v>
       </c>
-      <c r="O28" s="38">
+      <c r="O28" s="37">
         <v>38</v>
       </c>
-      <c r="P28" s="38" t="s">
+      <c r="P28" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="Q28" s="49" t="s">
+      <c r="Q28" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="R28" s="53"/>
+      <c r="R28" s="52"/>
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
       <c r="U28" s="10"/>
-      <c r="V28" s="57"/>
-      <c r="X28" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y28" s="53"/>
+      <c r="V28" s="56"/>
+      <c r="X28" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y28" s="52"/>
       <c r="Z28" s="10"/>
-      <c r="AA28" s="54"/>
+      <c r="AA28" s="53"/>
     </row>
     <row r="29" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L29" s="42"/>
-      <c r="M29" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="N29" s="37">
+      <c r="L29" s="41"/>
+      <c r="M29" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="N29" s="36">
         <v>39</v>
       </c>
-      <c r="O29" s="38">
+      <c r="O29" s="37">
         <v>40</v>
       </c>
-      <c r="P29" s="38" t="s">
+      <c r="P29" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="Q29" s="49" t="s">
+      <c r="Q29" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="R29" s="53"/>
+      <c r="R29" s="52"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>

</xml_diff>

<commit_message>
Tweaked the physical layout diagram a bit
</commit_message>
<xml_diff>
--- a/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
+++ b/PythonScale/DocsANdNotes/Data Flow and LEDs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="1"/>
+    <workbookView xWindow="8520" yWindow="0" windowWidth="19680" windowHeight="10350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LED Status" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="144">
   <si>
     <t>Power</t>
   </si>
@@ -446,6 +446,18 @@
   </si>
   <si>
     <t>LED - NoGo 3</t>
+  </si>
+  <si>
+    <t>LCD Pin 10</t>
+  </si>
+  <si>
+    <t>LCD Pin 7</t>
+  </si>
+  <si>
+    <t>LCD Pin 8</t>
+  </si>
+  <si>
+    <t>LCD Pin 9</t>
   </si>
 </sst>
 </file>
@@ -568,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -593,27 +605,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -644,41 +636,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -692,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,8 +668,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -813,15 +768,12 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1157,16 +1109,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
@@ -1186,16 +1138,16 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1215,12 +1167,12 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="5" t="s">
         <v>26</v>
       </c>
@@ -1231,12 +1183,12 @@
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="14"/>
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
@@ -1249,12 +1201,12 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
       <c r="F6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1272,12 +1224,12 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1290,10 +1242,10 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="6" t="s">
         <v>31</v>
       </c>
@@ -1306,10 +1258,10 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1329,12 +1281,12 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1349,12 +1301,12 @@
       <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1374,12 +1326,12 @@
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1397,12 +1349,12 @@
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -1431,7 +1383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
@@ -1464,16 +1416,16 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="16"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="16"/>
       <c r="F5" t="s">
         <v>109</v>
       </c>
@@ -1506,37 +1458,37 @@
       <c r="A6">
         <v>7</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>4</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="41" t="s">
+      <c r="F6" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="30">
         <v>1</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="31">
         <v>2</v>
       </c>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="K6" s="44" t="s">
+      <c r="K6" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="M6" s="37">
+      <c r="M6" s="35">
         <v>11</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="48" t="s">
+      <c r="O6" s="46" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1544,35 +1496,35 @@
       <c r="A7">
         <v>29</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>5</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="34" t="s">
+      <c r="F7" s="39"/>
+      <c r="G7" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="35">
+      <c r="H7" s="33">
         <v>3</v>
       </c>
-      <c r="I7" s="33">
+      <c r="I7" s="31">
         <v>4</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="M7" s="37">
+      <c r="M7" s="35">
         <v>13</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="O7" s="48" t="s">
+      <c r="O7" s="46" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1580,266 +1532,266 @@
       <c r="A8">
         <v>31</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>6</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="34" t="s">
+      <c r="F8" s="39"/>
+      <c r="G8" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="33">
         <v>5</v>
       </c>
-      <c r="I8" s="36">
+      <c r="I8" s="34">
         <v>6</v>
       </c>
-      <c r="J8" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" s="45" t="s">
+      <c r="J8" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="35">
         <v>15</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="48" t="s">
+      <c r="O8" s="46" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>7</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="22"/>
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="37" t="s">
+      <c r="F9" s="39"/>
+      <c r="G9" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="35">
         <v>7</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I9" s="36">
         <v>8</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="K9" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="30">
         <v>1</v>
       </c>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="O9" s="50" t="s">
+      <c r="O9" s="48" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
+      <c r="B10" s="21">
         <v>8</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="22"/>
       <c r="D10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H10" s="36">
+      <c r="G10" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="34">
         <v>9</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="36">
         <v>10</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="J10" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="K10" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="30">
         <v>17</v>
       </c>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="O10" s="50" t="s">
+      <c r="O10" s="48" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
+      <c r="B11" s="21">
         <v>9</v>
       </c>
-      <c r="C11" s="24"/>
+      <c r="C11" s="22"/>
       <c r="D11" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="35">
         <v>11</v>
       </c>
-      <c r="I11" s="37">
+      <c r="I11" s="35">
         <v>12</v>
       </c>
-      <c r="J11" s="37" t="s">
+      <c r="J11" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="47"/>
-      <c r="M11" s="36">
+      <c r="K11" s="45"/>
+      <c r="M11" s="34">
         <v>14</v>
       </c>
-      <c r="N11" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O11" s="51" t="s">
+      <c r="N11" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O11" s="49" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
+      <c r="B12" s="21">
         <v>10</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="22"/>
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="42" t="s">
+      <c r="F12" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="35">
         <v>13</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="34">
         <v>14</v>
       </c>
-      <c r="J12" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="45" t="s">
+      <c r="J12" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="31">
         <v>4</v>
       </c>
-      <c r="N12" s="33" t="s">
+      <c r="N12" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="42" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="23">
+      <c r="B13" s="21">
         <v>11</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="22"/>
       <c r="D13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="35">
         <v>15</v>
       </c>
-      <c r="I13" s="37">
+      <c r="I13" s="35">
         <v>16</v>
       </c>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="M13" s="31"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="47" t="s">
+      <c r="M13" s="29"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="45" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
+      <c r="B14" s="17">
         <v>12</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="F14" s="41" t="s">
+      <c r="C14" s="18"/>
+      <c r="F14" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="30">
         <v>17</v>
       </c>
-      <c r="I14" s="37">
+      <c r="I14" s="35">
         <v>18</v>
       </c>
-      <c r="J14" s="37" t="s">
+      <c r="J14" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="37">
+      <c r="M14" s="35">
         <v>16</v>
       </c>
-      <c r="N14" s="37" t="s">
+      <c r="N14" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="O14" s="48" t="s">
+      <c r="O14" s="46" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="17">
         <v>13</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="39" t="s">
+      <c r="C15" s="18"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="37">
         <v>19</v>
       </c>
-      <c r="I15" s="36">
+      <c r="I15" s="34">
         <v>20</v>
       </c>
-      <c r="J15" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K15" s="47"/>
-      <c r="M15" s="36">
+      <c r="J15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="45"/>
+      <c r="M15" s="34">
         <v>6</v>
       </c>
-      <c r="N15" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O15" s="45" t="s">
+      <c r="N15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="43" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1847,36 +1799,36 @@
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="19">
         <v>14</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="39" t="s">
+      <c r="F16" s="39"/>
+      <c r="G16" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="37">
         <v>21</v>
       </c>
-      <c r="I16" s="37">
+      <c r="I16" s="35">
         <v>22</v>
       </c>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="47"/>
-      <c r="M16" s="37">
+      <c r="K16" s="45"/>
+      <c r="M16" s="35">
         <v>18</v>
       </c>
-      <c r="N16" s="37" t="s">
+      <c r="N16" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="O16" s="48" t="s">
+      <c r="O16" s="46" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1884,36 +1836,36 @@
       <c r="A17">
         <v>10</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="19">
         <v>15</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="41"/>
-      <c r="G17" s="39" t="s">
+      <c r="F17" s="39"/>
+      <c r="G17" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="37">
         <v>23</v>
       </c>
-      <c r="I17" s="39">
+      <c r="I17" s="37">
         <v>24</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="K17" s="47"/>
-      <c r="M17" s="37">
+      <c r="K17" s="45"/>
+      <c r="M17" s="35">
         <v>32</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="N17" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="O17" s="48" t="s">
+      <c r="O17" s="46" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1921,33 +1873,33 @@
       <c r="A18">
         <v>36</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <v>16</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="41"/>
-      <c r="G18" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H18" s="36">
+      <c r="F18" s="39"/>
+      <c r="G18" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="34">
         <v>25</v>
       </c>
-      <c r="I18" s="39">
+      <c r="I18" s="37">
         <v>26</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="47"/>
-      <c r="M18" s="37">
+      <c r="K18" s="45"/>
+      <c r="M18" s="35">
         <v>36</v>
       </c>
-      <c r="N18" s="37" t="s">
+      <c r="N18" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="O18" s="48" t="s">
+      <c r="O18" s="46" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1955,33 +1907,33 @@
       <c r="A19">
         <v>11</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="17">
         <v>17</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="40" t="s">
+      <c r="F19" s="39"/>
+      <c r="G19" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="38">
         <v>27</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="38">
         <v>28</v>
       </c>
-      <c r="J19" s="40" t="s">
+      <c r="J19" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="K19" s="47"/>
-      <c r="M19" s="37">
+      <c r="K19" s="45"/>
+      <c r="M19" s="35">
         <v>38</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N19" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="O19" s="48" t="s">
+      <c r="O19" s="46" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1989,37 +1941,37 @@
       <c r="A20">
         <v>12</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="17">
         <v>18</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="42" t="s">
+      <c r="F20" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="35">
         <v>29</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="34">
         <v>30</v>
       </c>
-      <c r="J20" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K20" s="45" t="s">
+      <c r="J20" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K20" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="M20" s="37">
+      <c r="M20" s="35">
         <v>40</v>
       </c>
-      <c r="N20" s="37" t="s">
+      <c r="N20" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="O20" s="48" t="s">
+      <c r="O20" s="46" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2027,37 +1979,37 @@
       <c r="A21">
         <v>35</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <v>19</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="35">
         <v>31</v>
       </c>
-      <c r="I21" s="37">
+      <c r="I21" s="35">
         <v>32</v>
       </c>
-      <c r="J21" s="37" t="s">
+      <c r="J21" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="K21" s="48" t="s">
+      <c r="K21" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="31">
         <v>2</v>
       </c>
-      <c r="N21" s="33" t="s">
+      <c r="N21" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="O21" s="44" t="s">
+      <c r="O21" s="42" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2065,68 +2017,68 @@
       <c r="A22">
         <v>38</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>20</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="35">
         <v>33</v>
       </c>
-      <c r="I22" s="36">
+      <c r="I22" s="34">
         <v>34</v>
       </c>
-      <c r="J22" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="K22" s="43"/>
-      <c r="M22" s="36">
+      <c r="J22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K22" s="41"/>
+      <c r="M22" s="34">
         <v>30</v>
       </c>
-      <c r="N22" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O22" s="45" t="s">
+      <c r="N22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O22" s="43" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <v>21</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="F23" s="42" t="s">
+      <c r="C23" s="18"/>
+      <c r="F23" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="37" t="s">
+      <c r="G23" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="35">
         <v>35</v>
       </c>
-      <c r="I23" s="37">
+      <c r="I23" s="35">
         <v>36</v>
       </c>
-      <c r="J23" s="37" t="s">
+      <c r="J23" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="K23" s="48" t="s">
+      <c r="K23" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="M23" s="37">
+      <c r="M23" s="35">
         <v>31</v>
       </c>
-      <c r="N23" s="37" t="s">
+      <c r="N23" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="O23" s="48" t="s">
+      <c r="O23" s="46" t="s">
         <v>129</v>
       </c>
     </row>
@@ -2134,37 +2086,37 @@
       <c r="A24">
         <v>15</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <v>22</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="H24" s="37">
+      <c r="H24" s="35">
         <v>37</v>
       </c>
-      <c r="I24" s="37">
+      <c r="I24" s="35">
         <v>38</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="J24" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="K24" s="48" t="s">
+      <c r="K24" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="M24" s="37">
+      <c r="M24" s="35">
         <v>33</v>
       </c>
-      <c r="N24" s="37" t="s">
+      <c r="N24" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="O24" s="48" t="s">
+      <c r="O24" s="46" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2172,35 +2124,35 @@
       <c r="A25">
         <v>16</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>23</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="36">
+      <c r="F25" s="39"/>
+      <c r="G25" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="34">
         <v>39</v>
       </c>
-      <c r="I25" s="37">
+      <c r="I25" s="35">
         <v>40</v>
       </c>
-      <c r="J25" s="37" t="s">
+      <c r="J25" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="M25" s="37">
+      <c r="M25" s="35">
         <v>35</v>
       </c>
-      <c r="N25" s="37" t="s">
+      <c r="N25" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="O25" s="48" t="s">
+      <c r="O25" s="46" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2208,20 +2160,20 @@
       <c r="A26">
         <v>18</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="17">
         <v>24</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="K26" s="43"/>
-      <c r="M26" s="37">
+      <c r="K26" s="41"/>
+      <c r="M26" s="35">
         <v>37</v>
       </c>
-      <c r="N26" s="37" t="s">
+      <c r="N26" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="O26" s="48" t="s">
+      <c r="O26" s="46" t="s">
         <v>139</v>
       </c>
     </row>
@@ -2229,20 +2181,20 @@
       <c r="A27">
         <v>22</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="17">
         <v>25</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>54</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="M27" s="37">
+      <c r="M27" s="35">
         <v>29</v>
       </c>
-      <c r="N27" s="37" t="s">
+      <c r="N27" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="O27" s="48" t="s">
+      <c r="O27" s="46" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2250,20 +2202,20 @@
       <c r="A28">
         <v>37</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <v>26</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="18" t="s">
         <v>52</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="M28" s="38">
+      <c r="M28" s="36">
         <v>10</v>
       </c>
-      <c r="N28" s="38" t="s">
+      <c r="N28" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="O28" s="46" t="s">
+      <c r="O28" s="44" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2271,169 +2223,169 @@
       <c r="A29">
         <v>13</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="17">
         <v>27</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="18" t="s">
         <v>53</v>
       </c>
       <c r="K29" s="1"/>
-      <c r="M29" s="38">
+      <c r="M29" s="36">
         <v>8</v>
       </c>
-      <c r="N29" s="38" t="s">
+      <c r="N29" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="O29" s="46" t="s">
+      <c r="O29" s="44" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="K30" s="1"/>
-      <c r="M30" s="36">
+      <c r="M30" s="34">
         <v>9</v>
       </c>
-      <c r="N30" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O30" s="45"/>
+      <c r="N30" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O30" s="43"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>73</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="M31" s="36">
+      <c r="M31" s="34">
         <v>20</v>
       </c>
-      <c r="N31" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O31" s="45"/>
+      <c r="N31" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O31" s="43"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="25">
+      <c r="A32" s="23">
         <v>1</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="25" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="23" t="s">
         <v>76</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="M32" s="36">
+      <c r="M32" s="34">
         <v>25</v>
       </c>
-      <c r="N32" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O32" s="45"/>
+      <c r="N32" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O32" s="43"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="25">
+      <c r="A33" s="23">
         <v>17</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="25" t="s">
+      <c r="B33" s="24"/>
+      <c r="C33" s="23" t="s">
         <v>76</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="M33" s="36">
+      <c r="M33" s="34">
         <v>34</v>
       </c>
-      <c r="N33" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="O33" s="45"/>
+      <c r="N33" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="O33" s="43"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+      <c r="A34" s="27">
         <v>2</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="29" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="27" t="s">
         <v>75</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="M34" s="49">
+      <c r="M34" s="47">
         <v>39</v>
       </c>
-      <c r="N34" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="O34" s="51"/>
+      <c r="N34" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="O34" s="49"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
+      <c r="A35" s="27">
         <v>4</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="29" t="s">
+      <c r="B35" s="28"/>
+      <c r="C35" s="27" t="s">
         <v>75</v>
       </c>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="27">
+      <c r="A36" s="25">
         <v>6</v>
       </c>
-      <c r="B36" s="28"/>
-      <c r="C36" s="27" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="25" t="s">
         <v>74</v>
       </c>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
+      <c r="A37" s="25">
         <v>9</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="27" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="25" t="s">
         <v>74</v>
       </c>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="A38" s="25">
         <v>14</v>
       </c>
-      <c r="B38" s="28"/>
-      <c r="C38" s="27" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="27">
+      <c r="A39" s="25">
         <v>20</v>
       </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="27" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="27">
+      <c r="A40" s="25">
         <v>25</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="27" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="27">
+      <c r="A41" s="25">
         <v>30</v>
       </c>
-      <c r="B41" s="28"/>
-      <c r="C41" s="27" t="s">
+      <c r="B41" s="26"/>
+      <c r="C41" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+      <c r="A42" s="25">
         <v>39</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="27" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="25" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2448,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L10:AA29"/>
+  <dimension ref="L10:AA31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,489 +2413,502 @@
     <col min="14" max="15" width="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="4.7109375" customWidth="1"/>
+    <col min="18" max="23" width="3" customWidth="1"/>
     <col min="24" max="24" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="4.28515625" customWidth="1"/>
     <col min="26" max="26" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L10" s="41" t="s">
+      <c r="L10" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="32" t="s">
+      <c r="M10" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="30">
         <v>1</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="31">
         <v>2</v>
       </c>
-      <c r="P10" s="33" t="s">
+      <c r="P10" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="Q10" s="44" t="s">
+      <c r="Q10" s="42" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L11" s="41"/>
-      <c r="M11" s="34" t="s">
+      <c r="L11" s="39"/>
+      <c r="M11" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="33">
         <v>3</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="31">
         <v>4</v>
       </c>
-      <c r="P11" s="33" t="s">
+      <c r="P11" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="Q11" s="44" t="s">
+      <c r="Q11" s="42" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L12" s="41"/>
-      <c r="M12" s="34" t="s">
+      <c r="L12" s="39"/>
+      <c r="M12" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="N12" s="35">
+      <c r="N12" s="33">
         <v>5</v>
       </c>
-      <c r="O12" s="36">
+      <c r="O12" s="34">
         <v>6</v>
       </c>
-      <c r="P12" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q12" s="45" t="s">
+      <c r="P12" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q12" s="43" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="13" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L13" s="41"/>
-      <c r="M13" s="37" t="s">
+      <c r="L13" s="39"/>
+      <c r="M13" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="37">
+      <c r="N13" s="35">
         <v>7</v>
       </c>
-      <c r="O13" s="38">
+      <c r="O13" s="36">
         <v>8</v>
       </c>
-      <c r="P13" s="38" t="s">
+      <c r="P13" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="Q13" s="46" t="s">
+      <c r="Q13" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="X13" s="45" t="s">
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="M14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N14" s="34">
+        <v>9</v>
+      </c>
+      <c r="O14" s="36">
+        <v>10</v>
+      </c>
+      <c r="P14" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q14" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y14" s="50"/>
+      <c r="AA14" s="51"/>
+    </row>
+    <row r="15" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L15" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="M15" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="N15" s="35">
+        <v>11</v>
+      </c>
+      <c r="O15" s="35">
+        <v>12</v>
+      </c>
+      <c r="P15" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q15" s="45"/>
+      <c r="Z15" s="51"/>
+      <c r="AA15" s="51"/>
+    </row>
+    <row r="16" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L16" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="M16" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="N16" s="35">
+        <v>13</v>
+      </c>
+      <c r="O16" s="34">
+        <v>14</v>
+      </c>
+      <c r="P16" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q16" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="Y13" s="52"/>
-      <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="M14" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="N14" s="36">
-        <v>9</v>
-      </c>
-      <c r="O14" s="38">
-        <v>10</v>
-      </c>
-      <c r="P14" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q14" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="X14" s="44" t="s">
+      <c r="X16" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="51"/>
+    </row>
+    <row r="17" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L17" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="N17" s="35">
+        <v>15</v>
+      </c>
+      <c r="O17" s="35">
+        <v>16</v>
+      </c>
+      <c r="P17" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q17" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="X17" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="Y14" s="52"/>
-      <c r="AA14" s="53"/>
-    </row>
-    <row r="15" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L15" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="M15" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="N15" s="37">
-        <v>11</v>
-      </c>
-      <c r="O15" s="37">
-        <v>12</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q15" s="47"/>
-      <c r="X15" t="s">
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+    </row>
+    <row r="18" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L18" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="N18" s="30">
+        <v>17</v>
+      </c>
+      <c r="O18" s="35">
+        <v>18</v>
+      </c>
+      <c r="P18" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q18" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18" s="9"/>
+      <c r="T18" s="51"/>
+      <c r="X18" t="s">
         <v>137</v>
       </c>
-      <c r="Z15" s="53"/>
-      <c r="AA15" s="53"/>
-    </row>
-    <row r="16" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L16" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="M16" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="N16" s="37">
-        <v>13</v>
-      </c>
-      <c r="O16" s="36">
-        <v>14</v>
-      </c>
-      <c r="P16" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q16" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="48" t="s">
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+    </row>
+    <row r="19" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L19" s="39"/>
+      <c r="M19" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="N19" s="37">
+        <v>19</v>
+      </c>
+      <c r="O19" s="34">
+        <v>20</v>
+      </c>
+      <c r="P19" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q19" s="45"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="Z16" s="53"/>
-      <c r="AA16" s="53"/>
-    </row>
-    <row r="17" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L17" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="N17" s="37">
-        <v>15</v>
-      </c>
-      <c r="O17" s="37">
-        <v>16</v>
-      </c>
-      <c r="P17" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q17" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="R17" s="54"/>
-      <c r="X17" s="45" t="s">
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+    </row>
+    <row r="20" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L20" s="39"/>
+      <c r="M20" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="N20" s="37">
+        <v>21</v>
+      </c>
+      <c r="O20" s="35">
+        <v>22</v>
+      </c>
+      <c r="P20" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q20" s="45"/>
+      <c r="S20" s="51"/>
+      <c r="X20" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="Z17" s="53"/>
-      <c r="AA17" s="53"/>
-    </row>
-    <row r="18" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L18" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="M18" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="N18" s="32">
-        <v>17</v>
-      </c>
-      <c r="O18" s="37">
-        <v>18</v>
-      </c>
-      <c r="P18" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q18" s="48" t="s">
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+    </row>
+    <row r="21" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L21" s="39"/>
+      <c r="M21" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="N21" s="37">
+        <v>23</v>
+      </c>
+      <c r="O21" s="37">
+        <v>24</v>
+      </c>
+      <c r="P21" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q21" s="45"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z18" s="53"/>
-      <c r="AA18" s="53"/>
-    </row>
-    <row r="19" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L19" s="41"/>
-      <c r="M19" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="N19" s="39">
-        <v>19</v>
-      </c>
-      <c r="O19" s="36">
-        <v>20</v>
-      </c>
-      <c r="P19" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q19" s="47"/>
-      <c r="Z19" s="53"/>
-      <c r="AA19" s="53"/>
-    </row>
-    <row r="20" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L20" s="41"/>
-      <c r="M20" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="N20" s="39">
-        <v>21</v>
-      </c>
-      <c r="O20" s="37">
-        <v>22</v>
-      </c>
-      <c r="P20" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q20" s="47"/>
-      <c r="Z20" s="53"/>
-      <c r="AA20" s="53"/>
-    </row>
-    <row r="21" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L21" s="41"/>
-      <c r="M21" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="N21" s="39">
-        <v>23</v>
-      </c>
-      <c r="O21" s="39">
-        <v>24</v>
-      </c>
-      <c r="P21" s="39" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q21" s="47"/>
-      <c r="Z21" s="53"/>
-      <c r="AA21" s="53"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
     </row>
     <row r="22" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L22" s="41"/>
-      <c r="M22" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="N22" s="36">
+      <c r="L22" s="39"/>
+      <c r="M22" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" s="34">
         <v>25</v>
       </c>
-      <c r="O22" s="39">
+      <c r="O22" s="37">
         <v>26</v>
       </c>
-      <c r="P22" s="39" t="s">
+      <c r="P22" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="Q22" s="47"/>
-      <c r="Z22" s="53"/>
-      <c r="AA22" s="53"/>
+      <c r="Q22" s="45"/>
+      <c r="X22" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="51"/>
     </row>
     <row r="23" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L23" s="41"/>
-      <c r="M23" s="40" t="s">
+      <c r="L23" s="39"/>
+      <c r="M23" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="N23" s="40">
+      <c r="N23" s="38">
         <v>27</v>
       </c>
-      <c r="O23" s="40">
+      <c r="O23" s="38">
         <v>28</v>
       </c>
-      <c r="P23" s="40" t="s">
+      <c r="P23" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="Q23" s="47"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="48" t="s">
+      <c r="Q23" s="45"/>
+      <c r="X23" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+    </row>
+    <row r="24" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L24" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="M24" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="N24" s="35">
+        <v>29</v>
+      </c>
+      <c r="O24" s="34">
+        <v>30</v>
+      </c>
+      <c r="P24" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q24" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="R24" s="8"/>
+      <c r="X24" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="51"/>
+    </row>
+    <row r="25" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L25" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="M25" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="N25" s="35">
+        <v>31</v>
+      </c>
+      <c r="O25" s="35">
+        <v>32</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q25" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="Z23" s="53"/>
-      <c r="AA23" s="53"/>
-    </row>
-    <row r="24" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L24" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="M24" s="37" t="s">
-        <v>82</v>
-      </c>
-      <c r="N24" s="37">
-        <v>29</v>
-      </c>
-      <c r="O24" s="36">
-        <v>30</v>
-      </c>
-      <c r="P24" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q24" s="58" t="s">
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="X25" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="51"/>
+    </row>
+    <row r="26" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L26" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="N26" s="35">
+        <v>33</v>
+      </c>
+      <c r="O26" s="34">
+        <v>34</v>
+      </c>
+      <c r="P26" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q26" s="41"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="51"/>
+    </row>
+    <row r="27" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L27" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="M27" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="N27" s="35">
+        <v>35</v>
+      </c>
+      <c r="O27" s="35">
+        <v>36</v>
+      </c>
+      <c r="P27" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q27" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="R27" s="50"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y27" s="50"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="51"/>
+    </row>
+    <row r="28" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L28" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="N28" s="35">
+        <v>37</v>
+      </c>
+      <c r="O28" s="35">
+        <v>38</v>
+      </c>
+      <c r="P28" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q28" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="R28" s="50"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="51"/>
+    </row>
+    <row r="29" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="L29" s="39"/>
+      <c r="M29" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N29" s="34">
+        <v>39</v>
+      </c>
+      <c r="O29" s="35">
+        <v>40</v>
+      </c>
+      <c r="P29" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q29" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="R29" s="50"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="X30" s="42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="12:27" x14ac:dyDescent="0.25">
+      <c r="X31" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="R24" s="8"/>
-      <c r="S24" s="9"/>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z24" s="53"/>
-      <c r="AA24" s="53"/>
-    </row>
-    <row r="25" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L25" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="N25" s="37">
-        <v>31</v>
-      </c>
-      <c r="O25" s="37">
-        <v>32</v>
-      </c>
-      <c r="P25" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q25" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="R25" s="10"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="9"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z25" s="53"/>
-      <c r="AA25" s="53"/>
-    </row>
-    <row r="26" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L26" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="N26" s="37">
-        <v>33</v>
-      </c>
-      <c r="O26" s="36">
-        <v>34</v>
-      </c>
-      <c r="P26" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q26" s="43"/>
-      <c r="T26" s="9"/>
-      <c r="V26" s="55"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z26" s="53"/>
-      <c r="AA26" s="53"/>
-    </row>
-    <row r="27" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L27" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="M27" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="N27" s="37">
-        <v>35</v>
-      </c>
-      <c r="O27" s="37">
-        <v>36</v>
-      </c>
-      <c r="P27" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q27" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="R27" s="52"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="11"/>
-      <c r="V27" s="56"/>
-      <c r="X27" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y27" s="52"/>
-      <c r="Z27" s="53"/>
-      <c r="AA27" s="53"/>
-    </row>
-    <row r="28" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L28" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="M28" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="N28" s="37">
-        <v>37</v>
-      </c>
-      <c r="O28" s="37">
-        <v>38</v>
-      </c>
-      <c r="P28" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q28" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="R28" s="52"/>
-      <c r="S28" s="10"/>
-      <c r="T28" s="10"/>
-      <c r="U28" s="10"/>
-      <c r="V28" s="56"/>
-      <c r="X28" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="10"/>
-      <c r="AA28" s="53"/>
-    </row>
-    <row r="29" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="L29" s="41"/>
-      <c r="M29" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="N29" s="36">
-        <v>39</v>
-      </c>
-      <c r="O29" s="37">
-        <v>40</v>
-      </c>
-      <c r="P29" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q29" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="R29" s="52"/>
-      <c r="S29" s="10"/>
-      <c r="T29" s="10"/>
-      <c r="U29" s="10"/>
-      <c r="V29" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>